<commit_message>
Commit #2: | updated product backlog |
</commit_message>
<xml_diff>
--- a/Planning/Project Backlog.xlsx
+++ b/Planning/Project Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mediacollegeamsterdam-my.sharepoint.com/personal/31644_ma-web_nl/Documents/Bureaublad/Museum-Online/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4006155B-C828-43CC-ADE1-EFD4C116CB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{4006155B-C828-43CC-ADE1-EFD4C116CB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F40E2F01-C71F-4674-BC4A-F24D029F49FC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F2EB4A6-26D9-430D-927D-7818746629C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>TO-DO</t>
   </si>
@@ -174,15 +174,9 @@
     <t>om te zien waneer de museum open gaat</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>openingstijden erbij zetten</t>
   </si>
   <si>
-    <t>simpel</t>
-  </si>
-  <si>
     <t>informatie zien over de kunstenaar</t>
   </si>
   <si>
@@ -199,6 +193,30 @@
   </si>
   <si>
     <t>scrollbar bovenin de pagina zetten</t>
+  </si>
+  <si>
+    <t>zodat de klant ziet dat de website van het LAM is</t>
+  </si>
+  <si>
+    <t>een logo en tekst van het LAM</t>
+  </si>
+  <si>
+    <t>informatie over de museum zien</t>
+  </si>
+  <si>
+    <t>ze weten wat voor een museum het is</t>
+  </si>
+  <si>
+    <t>info tab hebben bij de foto van de museum</t>
+  </si>
+  <si>
+    <t>simpel design</t>
+  </si>
+  <si>
+    <t>de user de website makkelijk kan navigeren</t>
+  </si>
+  <si>
+    <t>niet veel dingen hebben op de website</t>
   </si>
 </sst>
 </file>
@@ -553,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35915D5-8C86-47D7-B534-474486435D69}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +583,7 @@
     <col min="3" max="3" width="37.7109375" customWidth="1"/>
     <col min="4" max="4" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="37" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -634,161 +652,246 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>15</v>
+      <c r="A8" t="s">
+        <v>6</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="1"/>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
       <c r="B15" t="s">
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
       <c r="C19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="1"/>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="1"/>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>51</v>
-      </c>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E24" s="1"/>
@@ -803,122 +906,19 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" t="s">
-        <v>37</v>
-      </c>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F29" t="s">
-        <v>35</v>
-      </c>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30" t="s">
-        <v>42</v>
-      </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" t="s">
-        <v>43</v>
-      </c>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="1"/>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commit #3 | Updated Product Backlog |
</commit_message>
<xml_diff>
--- a/Planning/Project Backlog.xlsx
+++ b/Planning/Project Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mediacollegeamsterdam-my.sharepoint.com/personal/31644_ma-web_nl/Documents/Bureaublad/Museum-Online/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{4006155B-C828-43CC-ADE1-EFD4C116CB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F40E2F01-C71F-4674-BC4A-F24D029F49FC}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{4006155B-C828-43CC-ADE1-EFD4C116CB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D2352C4E-2DE0-455D-8BA8-CBA420CEB792}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F2EB4A6-26D9-430D-927D-7818746629C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>TO-DO</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>niet veel dingen hebben op de website</t>
+  </si>
+  <si>
+    <t>logo en info over de museum hebben</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +660,12 @@
       <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">

</xml_diff>

<commit_message>
Commit #5 | Sprint 2 Backlog gemaakt | Updated product backlog |
</commit_message>
<xml_diff>
--- a/Planning/Project Backlog.xlsx
+++ b/Planning/Project Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mediacollegeamsterdam-my.sharepoint.com/personal/31644_ma-web_nl/Documents/Bureaublad/Museum-Online/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{4006155B-C828-43CC-ADE1-EFD4C116CB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D2352C4E-2DE0-455D-8BA8-CBA420CEB792}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{4006155B-C828-43CC-ADE1-EFD4C116CB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2770820-17CD-4440-8951-CD176EC6269C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F2EB4A6-26D9-430D-927D-7818746629C5}"/>
+    <workbookView xWindow="13545" yWindow="0" windowWidth="15210" windowHeight="13725" xr2:uid="{9F2EB4A6-26D9-430D-927D-7818746629C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>zodat</t>
   </si>
   <si>
-    <t>prioriteit</t>
-  </si>
-  <si>
     <t>hoe</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>logo en info over de museum hebben</t>
+  </si>
+  <si>
+    <t>size</t>
   </si>
 </sst>
 </file>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35915D5-8C86-47D7-B534-474486435D69}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,10 +604,10 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -618,70 +618,70 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -695,36 +695,36 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
         <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -735,36 +735,36 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
         <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
         <v>58</v>
-      </c>
-      <c r="D13" t="s">
-        <v>59</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -775,36 +775,36 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
         <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -815,87 +815,87 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>34</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
         <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
         <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
         <v>40</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
         <v>44</v>
-      </c>
-      <c r="D22" t="s">
-        <v>45</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit #7 | Added Materials | Updated Product Backlog |
</commit_message>
<xml_diff>
--- a/Planning/Project Backlog.xlsx
+++ b/Planning/Project Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mediacollegeamsterdam-my.sharepoint.com/personal/31644_ma-web_nl/Documents/Bureaublad/Museum-Online/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{4006155B-C828-43CC-ADE1-EFD4C116CB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2770820-17CD-4440-8951-CD176EC6269C}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{4006155B-C828-43CC-ADE1-EFD4C116CB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{37FAE295-ABA0-469B-BBA3-462035360586}"/>
   <bookViews>
-    <workbookView xWindow="13545" yWindow="0" windowWidth="15210" windowHeight="13725" xr2:uid="{9F2EB4A6-26D9-430D-927D-7818746629C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F2EB4A6-26D9-430D-927D-7818746629C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
   <si>
     <t>TO-DO</t>
   </si>
@@ -220,13 +220,22 @@
   </si>
   <si>
     <t>size</t>
+  </si>
+  <si>
+    <t>MoSCoW</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,16 +243,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -251,17 +281,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35915D5-8C86-47D7-B534-474486435D69}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,36 +637,40 @@
     <col min="1" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" customWidth="1"/>
     <col min="4" max="4" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -626,14 +682,17 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -643,14 +702,17 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -660,14 +722,17 @@
       <c r="D5" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -677,23 +742,28 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="G6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -703,14 +773,17 @@
       <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>31</v>
       </c>
@@ -720,18 +793,22 @@
       <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
@@ -743,14 +820,17 @@
       <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -760,18 +840,22 @@
       <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="F13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
@@ -783,14 +867,17 @@
       <c r="D15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>31</v>
       </c>
@@ -800,18 +887,22 @@
       <c r="D16" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="F16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
@@ -823,14 +914,17 @@
       <c r="D18" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>31</v>
       </c>
@@ -840,14 +934,17 @@
       <c r="D19" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -857,14 +954,17 @@
       <c r="D20" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>14</v>
       </c>
@@ -874,14 +974,17 @@
       <c r="D21" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>31</v>
       </c>
@@ -891,44 +994,50 @@
       <c r="D22" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E32" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit #8 | Updated website |
</commit_message>
<xml_diff>
--- a/Planning/Project Backlog.xlsx
+++ b/Planning/Project Backlog.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="90" documentId="8_{4006155B-C828-43CC-ADE1-EFD4C116CB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{37FAE295-ABA0-469B-BBA3-462035360586}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F2EB4A6-26D9-430D-927D-7818746629C5}"/>
+    <workbookView xWindow="1860" yWindow="2130" windowWidth="22935" windowHeight="11385" xr2:uid="{9F2EB4A6-26D9-430D-927D-7818746629C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35915D5-8C86-47D7-B534-474486435D69}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>